<commit_message>
datos de entrada y de salida
</commit_message>
<xml_diff>
--- a/src/main/resources/input/recetas.xlsx
+++ b/src/main/resources/input/recetas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\6003288\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse_workspace\receta-xml\receta-xml\src\main\resources\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BA2EE9A-A60D-4B1B-890C-5A6B379AB5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76F214A-1396-470D-86D8-6F65B3245F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{59C43549-5A90-4DA9-9B64-57C93A726BF0}"/>
   </bookViews>
@@ -54,28 +54,28 @@
     <t>Id</t>
   </si>
   <si>
-    <t>Sushi</t>
-  </si>
-  <si>
-    <t>Sushi Grade</t>
-  </si>
-  <si>
-    <t>Crab</t>
-  </si>
-  <si>
     <t>Patatas Queso</t>
   </si>
   <si>
-    <t>Potatoes</t>
-  </si>
-  <si>
     <t>Pollo</t>
   </si>
   <si>
-    <t>Chicken</t>
-  </si>
-  <si>
-    <t>Tomatoes</t>
+    <t>Patatas</t>
+  </si>
+  <si>
+    <t>Macarrones Con tomate</t>
+  </si>
+  <si>
+    <t>Macarrones</t>
+  </si>
+  <si>
+    <t>Tomate</t>
+  </si>
+  <si>
+    <t>Pollo con Queso</t>
+  </si>
+  <si>
+    <t>Queso</t>
   </si>
 </sst>
 </file>
@@ -118,9 +118,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,89 +440,91 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F4" sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.26953125" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" style="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="17.7265625" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3">
         <v>1</v>
       </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4">
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>2</v>
       </c>
     </row>

</xml_diff>